<commit_message>
lambda ans so on
</commit_message>
<xml_diff>
--- a/Python/Comments.xlsx
+++ b/Python/Comments.xlsx
@@ -283,13 +283,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이제 실험에 대한 설명이 끝났습니다.
-준비가 되시면, '스페이스 바' 를 눌러 다음으로 진행하시면 됩니다.
-혹시나 실험 과정에 대해서 이해가 되지 않는 부분이 있거나,
-궁금한 사항이 있으시면 담당자에게 설명을 요청하시기 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>세션 1
 세션 1에서 참여자께서는 "왼쪽"으로 제시되는 이야기에 집중하여야 합니다.
 오른쪽으로 제시되는 이야기는 무시하시면 됩니다.
@@ -310,12 +303,6 @@
     <t>세션 1이 끝났습니다.
 쉬는 시간입니다.
 충분히 휴식을 취한 뒤, '스페이스 바' 를 눌러 다음으로 진행해주세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세션 4가 끝났습니다.
-쉬는 시간입니다.
-충분히 휴식을 취한 뒤, 를 눌러 다음으로 진행해주세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -363,6 +350,19 @@
 3번 "오른쪽"으로 제시되는 이야기에 집중하셔야 합니다. 
 '세션 4' 에서는 각 이야기 쌍 별로 집중해야 햐는 방향이 "무작위"로 바뀝니다.
 각 세션에 대한 설명은 각 세션이 시작하기 전 다시 한 번 제공됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이제 실험에 대한 설명이 끝났습니다.
+준비가 되시면, '스페이스 바' 를 눌러 다음으로 진행하시면 됩니다.
+혹시나 실험 과정에 대해서 이해가 되지 않는 부분이 있거나,
+궁금한 사항이 있으시면 담당자에게 설명을 요청하시기 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 4가 끝났습니다.
+쉬는 시간입니다.
+충분히 휴식을 취한 뒤, '스페이스 바' 를 눌러 다음으로 진행해주세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -776,16 +776,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="261" x14ac:dyDescent="0.4">
@@ -842,7 +842,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
@@ -852,7 +852,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="243.6" x14ac:dyDescent="0.4">
@@ -860,7 +860,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>26</v>
@@ -874,7 +874,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>27</v>
@@ -902,7 +902,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>29</v>
@@ -913,17 +913,17 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="174" x14ac:dyDescent="0.4">
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>